<commit_message>
u bv corpus xlsx
</commit_message>
<xml_diff>
--- a/txt/bipoc-voices-corpus/data/bipoc-voices-corpus-metadata.xlsx
+++ b/txt/bipoc-voices-corpus/data/bipoc-voices-corpus-metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/onemorevoice/txt/bipoc-voices-corpus/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDABD44-D5C6-C844-9668-E896E0AD629C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C10ED0-338B-EA43-BBA8-9A29DEDDB144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="460" windowWidth="24900" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="495">
   <si>
     <t>OMV identifier</t>
   </si>
@@ -1505,6 +1505,54 @@
   </si>
   <si>
     <t>AMD URL</t>
+  </si>
+  <si>
+    <t>liv_025997</t>
+  </si>
+  <si>
+    <t>liv_025998</t>
+  </si>
+  <si>
+    <t>liv_025999</t>
+  </si>
+  <si>
+    <t>Selim Aga</t>
+  </si>
+  <si>
+    <t>The Geographical Journal</t>
+  </si>
+  <si>
+    <t>A Trip Up the Congo or Zaire River</t>
+  </si>
+  <si>
+    <t>1 July 1875</t>
+  </si>
+  <si>
+    <t>1875-07-01</t>
+  </si>
+  <si>
+    <t>203-07</t>
+  </si>
+  <si>
+    <t>West and Central Africa</t>
+  </si>
+  <si>
+    <t>My Parentage and Early Career as a Slave</t>
+  </si>
+  <si>
+    <t>63-69; 120</t>
+  </si>
+  <si>
+    <t>Africa Considered in its Social and Political Condition [...]</t>
+  </si>
+  <si>
+    <t>1853-05</t>
+  </si>
+  <si>
+    <t>May 1853</t>
+  </si>
+  <si>
+    <t>short book</t>
   </si>
 </sst>
 </file>
@@ -2096,11 +2144,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z731"/>
+  <dimension ref="A1:Z735"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3164,272 +3212,206 @@
       <c r="N23" s="50"/>
       <c r="O23" s="52"/>
       <c r="P23" s="52"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
-      <c r="U23" s="5"/>
-      <c r="V23" s="5"/>
-      <c r="W23" s="5"/>
-    </row>
-    <row r="24" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="G24" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="H24" s="20">
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13"/>
+      <c r="W23" s="13"/>
+    </row>
+    <row r="24" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
+        <v>479</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>482</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13" t="s">
+        <v>491</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="H24" s="13"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13" t="s">
+        <v>488</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>494</v>
+      </c>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13"/>
+      <c r="W24" s="13"/>
+    </row>
+    <row r="25" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
+        <v>480</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>482</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>483</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H25" s="12">
         <v>1</v>
       </c>
-      <c r="I24" s="20">
-        <v>1</v>
-      </c>
-      <c r="J24" s="23">
-        <v>44480</v>
-      </c>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="M24" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="N24" s="12"/>
-      <c r="O24" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="P24" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q24" s="20"/>
-      <c r="R24" s="20"/>
-      <c r="S24" s="20"/>
-      <c r="T24" s="20"/>
-      <c r="U24" s="20"/>
-      <c r="V24" s="20"/>
-      <c r="W24" s="24"/>
-      <c r="X24" s="24"/>
-      <c r="Y24" s="24"/>
-      <c r="Z24" s="24"/>
-    </row>
-    <row r="25" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A25" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="G25" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="H25" s="20">
-        <v>1</v>
-      </c>
-      <c r="I25" s="20">
-        <v>13</v>
-      </c>
-      <c r="J25" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="M25" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="N25" s="12"/>
-      <c r="O25" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="P25" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="20"/>
-      <c r="S25" s="20"/>
-      <c r="T25" s="20"/>
-      <c r="U25" s="20"/>
-      <c r="V25" s="20"/>
-      <c r="W25" s="24"/>
-      <c r="X25" s="24"/>
-      <c r="Y25" s="24"/>
-      <c r="Z25" s="24"/>
-    </row>
-    <row r="26" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A26" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="F26" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="G26" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="H26" s="20">
-        <v>1</v>
-      </c>
-      <c r="I26" s="20">
-        <v>14</v>
-      </c>
-      <c r="J26" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="M26" s="20" t="s">
-        <v>209</v>
-      </c>
-      <c r="N26" s="12"/>
-      <c r="O26" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="P26" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="20"/>
-      <c r="S26" s="20"/>
-      <c r="T26" s="20"/>
-      <c r="U26" s="20"/>
-      <c r="V26" s="20"/>
-      <c r="W26" s="24"/>
-      <c r="X26" s="24"/>
-      <c r="Y26" s="24"/>
-      <c r="Z26" s="24"/>
-    </row>
-    <row r="27" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A27" s="19" t="s">
-        <v>211</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="F27" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="G27" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="H27" s="20">
-        <v>1</v>
-      </c>
-      <c r="I27" s="20">
-        <v>14</v>
-      </c>
-      <c r="J27" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="M27" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="N27" s="12"/>
-      <c r="O27" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="P27" s="20" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="20"/>
-      <c r="S27" s="20"/>
-      <c r="T27" s="20"/>
-      <c r="U27" s="20"/>
-      <c r="V27" s="20"/>
-      <c r="W27" s="24"/>
-      <c r="X27" s="24"/>
-      <c r="Y27" s="24"/>
-      <c r="Z27" s="24"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="12" t="s">
+        <v>490</v>
+      </c>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13" t="s">
+        <v>488</v>
+      </c>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="13"/>
+      <c r="W25" s="13"/>
+    </row>
+    <row r="26" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
+        <v>481</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>482</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13" t="s">
+        <v>484</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>483</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="H26" s="12">
+        <v>2</v>
+      </c>
+      <c r="I26" s="16"/>
+      <c r="J26" s="12" t="s">
+        <v>487</v>
+      </c>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13" t="s">
+        <v>488</v>
+      </c>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="13"/>
+      <c r="W26" s="13"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A27" s="50"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="52"/>
+      <c r="P27" s="52"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
     </row>
     <row r="28" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="C28" s="20"/>
       <c r="D28" s="20" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="E28" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>219</v>
+        <v>190</v>
       </c>
       <c r="G28" s="22" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
       <c r="H28" s="20">
         <v>1</v>
       </c>
       <c r="I28" s="20">
-        <v>17</v>
-      </c>
-      <c r="J28" s="20" t="s">
-        <v>221</v>
+        <v>1</v>
+      </c>
+      <c r="J28" s="23">
+        <v>44480</v>
       </c>
       <c r="K28" s="20"/>
       <c r="L28" s="20" t="s">
         <v>188</v>
       </c>
       <c r="M28" s="20" t="s">
-        <v>222</v>
+        <v>192</v>
       </c>
       <c r="N28" s="12"/>
       <c r="O28" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P28" s="20" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="Q28" s="20"/>
       <c r="R28" s="20"/>
@@ -3444,46 +3426,46 @@
     </row>
     <row r="29" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>225</v>
+        <v>196</v>
       </c>
       <c r="C29" s="20"/>
       <c r="D29" s="20" t="s">
-        <v>226</v>
+        <v>197</v>
       </c>
       <c r="E29" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>227</v>
+        <v>198</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>228</v>
+        <v>199</v>
       </c>
       <c r="H29" s="20">
         <v>1</v>
       </c>
       <c r="I29" s="20">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J29" s="20" t="s">
-        <v>229</v>
+        <v>200</v>
       </c>
       <c r="K29" s="20"/>
       <c r="L29" s="20" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="M29" s="20" t="s">
-        <v>230</v>
+        <v>201</v>
       </c>
       <c r="N29" s="12"/>
       <c r="O29" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P29" s="20" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
       <c r="Q29" s="20"/>
       <c r="R29" s="20"/>
@@ -3498,44 +3480,46 @@
     </row>
     <row r="30" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
-        <v>232</v>
+        <v>203</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>233</v>
+        <v>42</v>
       </c>
       <c r="C30" s="20"/>
       <c r="D30" s="20" t="s">
-        <v>234</v>
+        <v>204</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>235</v>
+        <v>189</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="G30" s="22" t="s">
-        <v>237</v>
-      </c>
-      <c r="H30" s="20"/>
+        <v>206</v>
+      </c>
+      <c r="H30" s="20">
+        <v>1</v>
+      </c>
       <c r="I30" s="20">
-        <v>1</v>
-      </c>
-      <c r="J30" s="20">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="J30" s="20" t="s">
+        <v>207</v>
       </c>
       <c r="K30" s="20"/>
       <c r="L30" s="20" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="M30" s="20" t="s">
-        <v>239</v>
+        <v>209</v>
       </c>
       <c r="N30" s="12"/>
       <c r="O30" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P30" s="20" t="s">
-        <v>240</v>
+        <v>210</v>
       </c>
       <c r="Q30" s="20"/>
       <c r="R30" s="20"/>
@@ -3550,46 +3534,46 @@
     </row>
     <row r="31" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="C31" s="20"/>
       <c r="D31" s="20" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>244</v>
+        <v>189</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>245</v>
+        <v>205</v>
       </c>
       <c r="G31" s="22" t="s">
-        <v>246</v>
+        <v>206</v>
       </c>
       <c r="H31" s="20">
         <v>1</v>
       </c>
       <c r="I31" s="20">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="J31" s="20" t="s">
-        <v>247</v>
+        <v>123</v>
       </c>
       <c r="K31" s="20"/>
       <c r="L31" s="20" t="s">
-        <v>248</v>
+        <v>45</v>
       </c>
       <c r="M31" s="20" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="N31" s="12"/>
       <c r="O31" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P31" s="20" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="Q31" s="20"/>
       <c r="R31" s="20"/>
@@ -3602,48 +3586,48 @@
       <c r="Y31" s="24"/>
       <c r="Z31" s="24"/>
     </row>
-    <row r="32" spans="1:26" s="25" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
-        <v>251</v>
+        <v>216</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>252</v>
+        <v>217</v>
       </c>
       <c r="C32" s="20"/>
       <c r="D32" s="20" t="s">
-        <v>253</v>
+        <v>218</v>
       </c>
       <c r="E32" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>254</v>
+        <v>219</v>
       </c>
       <c r="G32" s="22" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="H32" s="20">
         <v>1</v>
       </c>
       <c r="I32" s="20">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J32" s="20" t="s">
-        <v>256</v>
+        <v>221</v>
       </c>
       <c r="K32" s="20"/>
       <c r="L32" s="20" t="s">
-        <v>65</v>
+        <v>188</v>
       </c>
       <c r="M32" s="20" t="s">
-        <v>257</v>
+        <v>222</v>
       </c>
       <c r="N32" s="12"/>
       <c r="O32" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P32" s="20" t="s">
-        <v>258</v>
+        <v>223</v>
       </c>
       <c r="Q32" s="20"/>
       <c r="R32" s="20"/>
@@ -3656,48 +3640,48 @@
       <c r="Y32" s="24"/>
       <c r="Z32" s="24"/>
     </row>
-    <row r="33" spans="1:26" s="25" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
-        <v>259</v>
+        <v>224</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>260</v>
+        <v>225</v>
       </c>
       <c r="C33" s="20"/>
       <c r="D33" s="20" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
       <c r="E33" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>262</v>
+        <v>227</v>
       </c>
       <c r="G33" s="22" t="s">
-        <v>263</v>
+        <v>228</v>
       </c>
       <c r="H33" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33" s="20">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="J33" s="20" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="K33" s="20"/>
       <c r="L33" s="20" t="s">
-        <v>265</v>
+        <v>208</v>
       </c>
       <c r="M33" s="20" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="N33" s="12"/>
       <c r="O33" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P33" s="20" t="s">
-        <v>267</v>
+        <v>231</v>
       </c>
       <c r="Q33" s="20"/>
       <c r="R33" s="20"/>
@@ -3712,46 +3696,44 @@
     </row>
     <row r="34" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
-        <v>268</v>
+        <v>232</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>269</v>
+        <v>233</v>
       </c>
       <c r="C34" s="20"/>
       <c r="D34" s="20" t="s">
-        <v>270</v>
+        <v>234</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>271</v>
+        <v>236</v>
       </c>
       <c r="G34" s="22" t="s">
-        <v>272</v>
-      </c>
-      <c r="H34" s="20">
-        <v>2</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="H34" s="20"/>
       <c r="I34" s="20">
+        <v>1</v>
+      </c>
+      <c r="J34" s="20">
         <v>4</v>
-      </c>
-      <c r="J34" s="20" t="s">
-        <v>114</v>
       </c>
       <c r="K34" s="20"/>
       <c r="L34" s="20" t="s">
-        <v>45</v>
+        <v>238</v>
       </c>
       <c r="M34" s="20" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="N34" s="12"/>
       <c r="O34" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P34" s="20" t="s">
-        <v>273</v>
+        <v>240</v>
       </c>
       <c r="Q34" s="20"/>
       <c r="R34" s="20"/>
@@ -3764,48 +3746,48 @@
       <c r="Y34" s="24"/>
       <c r="Z34" s="24"/>
     </row>
-    <row r="35" spans="1:26" s="25" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
-        <v>274</v>
+        <v>241</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>275</v>
+        <v>242</v>
       </c>
       <c r="C35" s="20"/>
       <c r="D35" s="20" t="s">
-        <v>276</v>
+        <v>243</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>189</v>
+        <v>244</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>277</v>
+        <v>245</v>
       </c>
       <c r="G35" s="22" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
       <c r="H35" s="20">
+        <v>1</v>
+      </c>
+      <c r="I35" s="20">
         <v>2</v>
       </c>
-      <c r="I35" s="20">
-        <v>6</v>
-      </c>
       <c r="J35" s="20" t="s">
-        <v>279</v>
+        <v>247</v>
       </c>
       <c r="K35" s="20"/>
       <c r="L35" s="20" t="s">
-        <v>45</v>
+        <v>248</v>
       </c>
       <c r="M35" s="20" t="s">
-        <v>280</v>
+        <v>249</v>
       </c>
       <c r="N35" s="12"/>
       <c r="O35" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P35" s="20" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
       <c r="Q35" s="20"/>
       <c r="R35" s="20"/>
@@ -3818,48 +3800,48 @@
       <c r="Y35" s="24"/>
       <c r="Z35" s="24"/>
     </row>
-    <row r="36" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" s="25" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
-        <v>282</v>
+        <v>251</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>283</v>
+        <v>252</v>
       </c>
       <c r="C36" s="20"/>
       <c r="D36" s="20" t="s">
-        <v>284</v>
+        <v>253</v>
       </c>
       <c r="E36" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="G36" s="22" t="s">
-        <v>286</v>
+        <v>255</v>
       </c>
       <c r="H36" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I36" s="20">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="J36" s="20" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
       <c r="K36" s="20"/>
       <c r="L36" s="20" t="s">
-        <v>288</v>
+        <v>65</v>
       </c>
       <c r="M36" s="20" t="s">
-        <v>289</v>
+        <v>257</v>
       </c>
       <c r="N36" s="12"/>
       <c r="O36" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P36" s="20" t="s">
-        <v>290</v>
+        <v>258</v>
       </c>
       <c r="Q36" s="20"/>
       <c r="R36" s="20"/>
@@ -3872,48 +3854,48 @@
       <c r="Y36" s="24"/>
       <c r="Z36" s="24"/>
     </row>
-    <row r="37" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" s="25" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
-        <v>291</v>
+        <v>259</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>292</v>
+        <v>260</v>
       </c>
       <c r="C37" s="20"/>
       <c r="D37" s="20" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
       <c r="E37" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="G37" s="22" t="s">
-        <v>286</v>
+        <v>263</v>
       </c>
       <c r="H37" s="20">
         <v>2</v>
       </c>
       <c r="I37" s="20">
-        <v>10</v>
-      </c>
-      <c r="J37" s="20">
-        <v>114</v>
+        <v>3</v>
+      </c>
+      <c r="J37" s="20" t="s">
+        <v>264</v>
       </c>
       <c r="K37" s="20"/>
       <c r="L37" s="20" t="s">
-        <v>208</v>
+        <v>265</v>
       </c>
       <c r="M37" s="20" t="s">
-        <v>294</v>
+        <v>266</v>
       </c>
       <c r="N37" s="12"/>
       <c r="O37" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P37" s="20" t="s">
-        <v>295</v>
+        <v>267</v>
       </c>
       <c r="Q37" s="20"/>
       <c r="R37" s="20"/>
@@ -3928,46 +3910,46 @@
     </row>
     <row r="38" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
-        <v>296</v>
+        <v>268</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>297</v>
+        <v>269</v>
       </c>
       <c r="C38" s="20"/>
       <c r="D38" s="20" t="s">
-        <v>298</v>
+        <v>270</v>
       </c>
       <c r="E38" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="G38" s="22" t="s">
-        <v>300</v>
+        <v>272</v>
       </c>
       <c r="H38" s="20">
         <v>2</v>
       </c>
       <c r="I38" s="20">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J38" s="20" t="s">
-        <v>301</v>
+        <v>114</v>
       </c>
       <c r="K38" s="20"/>
       <c r="L38" s="20" t="s">
-        <v>188</v>
+        <v>45</v>
       </c>
       <c r="M38" s="20" t="s">
-        <v>302</v>
+        <v>230</v>
       </c>
       <c r="N38" s="12"/>
       <c r="O38" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P38" s="20" t="s">
-        <v>303</v>
+        <v>273</v>
       </c>
       <c r="Q38" s="20"/>
       <c r="R38" s="20"/>
@@ -3980,48 +3962,48 @@
       <c r="Y38" s="24"/>
       <c r="Z38" s="24"/>
     </row>
-    <row r="39" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" s="25" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="B39" s="26" t="s">
-        <v>297</v>
+        <v>274</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>275</v>
       </c>
       <c r="C39" s="20"/>
       <c r="D39" s="20" t="s">
-        <v>298</v>
-      </c>
-      <c r="E39" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="E39" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="G39" s="22" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="H39" s="20">
         <v>2</v>
       </c>
       <c r="I39" s="20">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J39" s="20" t="s">
-        <v>305</v>
+        <v>279</v>
       </c>
       <c r="K39" s="20"/>
       <c r="L39" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="M39" s="26" t="s">
-        <v>306</v>
+        <v>45</v>
+      </c>
+      <c r="M39" s="20" t="s">
+        <v>280</v>
       </c>
       <c r="N39" s="12"/>
       <c r="O39" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P39" s="20" t="s">
-        <v>307</v>
+        <v>281</v>
       </c>
       <c r="Q39" s="20"/>
       <c r="R39" s="20"/>
@@ -4036,46 +4018,46 @@
     </row>
     <row r="40" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
-        <v>308</v>
-      </c>
-      <c r="B40" s="26" t="s">
-        <v>297</v>
+        <v>282</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>283</v>
       </c>
       <c r="C40" s="20"/>
       <c r="D40" s="20" t="s">
-        <v>298</v>
-      </c>
-      <c r="E40" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="E40" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>309</v>
+        <v>285</v>
       </c>
       <c r="G40" s="22" t="s">
-        <v>310</v>
+        <v>286</v>
       </c>
       <c r="H40" s="20">
         <v>2</v>
       </c>
       <c r="I40" s="20">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J40" s="20" t="s">
-        <v>311</v>
+        <v>287</v>
       </c>
       <c r="K40" s="20"/>
       <c r="L40" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="M40" s="26" t="s">
-        <v>312</v>
+        <v>288</v>
+      </c>
+      <c r="M40" s="20" t="s">
+        <v>289</v>
       </c>
       <c r="N40" s="12"/>
       <c r="O40" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P40" s="20" t="s">
-        <v>313</v>
+        <v>290</v>
       </c>
       <c r="Q40" s="20"/>
       <c r="R40" s="20"/>
@@ -4090,46 +4072,46 @@
     </row>
     <row r="41" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
-        <v>314</v>
-      </c>
-      <c r="B41" s="26" t="s">
-        <v>297</v>
+        <v>291</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>292</v>
       </c>
       <c r="C41" s="20"/>
       <c r="D41" s="20" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E41" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>315</v>
+        <v>285</v>
       </c>
       <c r="G41" s="22" t="s">
-        <v>316</v>
+        <v>286</v>
       </c>
       <c r="H41" s="20">
         <v>2</v>
       </c>
       <c r="I41" s="20">
-        <v>12</v>
-      </c>
-      <c r="J41" s="20" t="s">
-        <v>317</v>
+        <v>10</v>
+      </c>
+      <c r="J41" s="20">
+        <v>114</v>
       </c>
       <c r="K41" s="20"/>
       <c r="L41" s="20" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="M41" s="20" t="s">
-        <v>318</v>
+        <v>294</v>
       </c>
       <c r="N41" s="12"/>
       <c r="O41" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P41" s="20" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="Q41" s="20"/>
       <c r="R41" s="20"/>
@@ -4144,46 +4126,46 @@
     </row>
     <row r="42" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="C42" s="20"/>
       <c r="D42" s="20" t="s">
-        <v>322</v>
+        <v>298</v>
       </c>
       <c r="E42" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>323</v>
+        <v>299</v>
       </c>
       <c r="G42" s="22" t="s">
-        <v>324</v>
+        <v>300</v>
       </c>
       <c r="H42" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I42" s="20">
-        <v>6</v>
-      </c>
-      <c r="J42" s="20">
-        <v>66</v>
+        <v>9</v>
+      </c>
+      <c r="J42" s="20" t="s">
+        <v>301</v>
       </c>
       <c r="K42" s="20"/>
       <c r="L42" s="20" t="s">
         <v>188</v>
       </c>
       <c r="M42" s="20" t="s">
-        <v>325</v>
+        <v>302</v>
       </c>
       <c r="N42" s="12"/>
       <c r="O42" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P42" s="20" t="s">
-        <v>326</v>
+        <v>303</v>
       </c>
       <c r="Q42" s="20"/>
       <c r="R42" s="20"/>
@@ -4198,46 +4180,46 @@
     </row>
     <row r="43" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
-        <v>327</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>328</v>
+        <v>304</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>297</v>
       </c>
       <c r="C43" s="20"/>
       <c r="D43" s="20" t="s">
-        <v>329</v>
-      </c>
-      <c r="E43" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="E43" s="26" t="s">
         <v>189</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>330</v>
+        <v>285</v>
       </c>
       <c r="G43" s="22" t="s">
-        <v>331</v>
+        <v>286</v>
       </c>
       <c r="H43" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I43" s="20">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J43" s="20" t="s">
-        <v>332</v>
+        <v>305</v>
       </c>
       <c r="K43" s="20"/>
       <c r="L43" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="M43" s="20" t="s">
-        <v>333</v>
+        <v>188</v>
+      </c>
+      <c r="M43" s="26" t="s">
+        <v>306</v>
       </c>
       <c r="N43" s="12"/>
       <c r="O43" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P43" s="20" t="s">
-        <v>334</v>
+        <v>307</v>
       </c>
       <c r="Q43" s="20"/>
       <c r="R43" s="20"/>
@@ -4252,46 +4234,46 @@
     </row>
     <row r="44" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
-        <v>335</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>336</v>
+        <v>308</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>297</v>
       </c>
       <c r="C44" s="20"/>
       <c r="D44" s="20" t="s">
-        <v>337</v>
-      </c>
-      <c r="E44" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="E44" s="26" t="s">
         <v>189</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>338</v>
+        <v>309</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>339</v>
+        <v>310</v>
       </c>
       <c r="H44" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I44" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J44" s="20" t="s">
-        <v>105</v>
+        <v>311</v>
       </c>
       <c r="K44" s="20"/>
       <c r="L44" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="M44" s="20" t="s">
-        <v>340</v>
+        <v>188</v>
+      </c>
+      <c r="M44" s="26" t="s">
+        <v>312</v>
       </c>
       <c r="N44" s="12"/>
       <c r="O44" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P44" s="20" t="s">
-        <v>341</v>
+        <v>313</v>
       </c>
       <c r="Q44" s="20"/>
       <c r="R44" s="20"/>
@@ -4306,46 +4288,46 @@
     </row>
     <row r="45" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
-        <v>342</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>343</v>
+        <v>314</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>297</v>
       </c>
       <c r="C45" s="20"/>
       <c r="D45" s="20" t="s">
-        <v>344</v>
+        <v>298</v>
       </c>
       <c r="E45" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>345</v>
+        <v>315</v>
       </c>
       <c r="G45" s="22" t="s">
-        <v>346</v>
+        <v>316</v>
       </c>
       <c r="H45" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I45" s="20">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J45" s="20" t="s">
-        <v>347</v>
+        <v>317</v>
       </c>
       <c r="K45" s="20"/>
       <c r="L45" s="20" t="s">
-        <v>348</v>
+        <v>188</v>
       </c>
       <c r="M45" s="20" t="s">
-        <v>349</v>
+        <v>318</v>
       </c>
       <c r="N45" s="12"/>
       <c r="O45" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P45" s="20" t="s">
-        <v>350</v>
+        <v>319</v>
       </c>
       <c r="Q45" s="20"/>
       <c r="R45" s="20"/>
@@ -4360,46 +4342,46 @@
     </row>
     <row r="46" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
-        <v>351</v>
+        <v>320</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>352</v>
+        <v>321</v>
       </c>
       <c r="C46" s="20"/>
       <c r="D46" s="20" t="s">
-        <v>353</v>
+        <v>322</v>
       </c>
       <c r="E46" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F46" s="21" t="s">
-        <v>354</v>
+        <v>323</v>
       </c>
       <c r="G46" s="22" t="s">
-        <v>355</v>
+        <v>324</v>
       </c>
       <c r="H46" s="20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I46" s="20">
         <v>6</v>
       </c>
-      <c r="J46" s="20" t="s">
-        <v>356</v>
+      <c r="J46" s="20">
+        <v>66</v>
       </c>
       <c r="K46" s="20"/>
       <c r="L46" s="20" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="M46" s="20" t="s">
-        <v>357</v>
+        <v>325</v>
       </c>
       <c r="N46" s="12"/>
       <c r="O46" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P46" s="20" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="Q46" s="20"/>
       <c r="R46" s="20"/>
@@ -4414,46 +4396,46 @@
     </row>
     <row r="47" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>360</v>
+        <v>328</v>
       </c>
       <c r="C47" s="20"/>
       <c r="D47" s="20" t="s">
-        <v>361</v>
+        <v>329</v>
       </c>
       <c r="E47" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F47" s="21" t="s">
-        <v>362</v>
+        <v>330</v>
       </c>
       <c r="G47" s="22" t="s">
-        <v>363</v>
+        <v>331</v>
       </c>
       <c r="H47" s="20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I47" s="20">
         <v>7</v>
       </c>
       <c r="J47" s="20" t="s">
-        <v>106</v>
+        <v>332</v>
       </c>
       <c r="K47" s="20"/>
       <c r="L47" s="20" t="s">
-        <v>208</v>
+        <v>45</v>
       </c>
       <c r="M47" s="20" t="s">
-        <v>364</v>
+        <v>333</v>
       </c>
       <c r="N47" s="12"/>
       <c r="O47" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P47" s="20" t="s">
-        <v>365</v>
+        <v>334</v>
       </c>
       <c r="Q47" s="20"/>
       <c r="R47" s="20"/>
@@ -4468,46 +4450,46 @@
     </row>
     <row r="48" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="s">
-        <v>366</v>
+        <v>335</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>367</v>
+        <v>336</v>
       </c>
       <c r="C48" s="20"/>
       <c r="D48" s="20" t="s">
-        <v>368</v>
+        <v>337</v>
       </c>
       <c r="E48" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>131</v>
+        <v>338</v>
       </c>
       <c r="G48" s="22" t="s">
-        <v>132</v>
+        <v>339</v>
       </c>
       <c r="H48" s="20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I48" s="20">
-        <v>3</v>
-      </c>
-      <c r="J48" s="20">
-        <v>26</v>
+        <v>9</v>
+      </c>
+      <c r="J48" s="20" t="s">
+        <v>105</v>
       </c>
       <c r="K48" s="20"/>
       <c r="L48" s="20" t="s">
         <v>45</v>
       </c>
       <c r="M48" s="20" t="s">
-        <v>369</v>
+        <v>340</v>
       </c>
       <c r="N48" s="12"/>
       <c r="O48" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P48" s="20" t="s">
-        <v>370</v>
+        <v>341</v>
       </c>
       <c r="Q48" s="20"/>
       <c r="R48" s="20"/>
@@ -4522,50 +4504,46 @@
     </row>
     <row r="49" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="19" t="s">
-        <v>371</v>
+        <v>342</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>372</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>373</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="C49" s="20"/>
       <c r="D49" s="20" t="s">
-        <v>374</v>
+        <v>344</v>
       </c>
       <c r="E49" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F49" s="21" t="s">
-        <v>133</v>
+        <v>345</v>
       </c>
       <c r="G49" s="22" t="s">
-        <v>134</v>
+        <v>346</v>
       </c>
       <c r="H49" s="20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I49" s="20">
-        <v>4</v>
-      </c>
-      <c r="J49" s="20">
-        <v>39</v>
-      </c>
-      <c r="K49" s="20">
-        <v>2</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="J49" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="K49" s="20"/>
       <c r="L49" s="20" t="s">
-        <v>65</v>
+        <v>348</v>
       </c>
       <c r="M49" s="20" t="s">
-        <v>375</v>
+        <v>349</v>
       </c>
       <c r="N49" s="12"/>
       <c r="O49" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P49" s="20" t="s">
-        <v>376</v>
+        <v>350</v>
       </c>
       <c r="Q49" s="20"/>
       <c r="R49" s="20"/>
@@ -4580,48 +4558,46 @@
     </row>
     <row r="50" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="s">
-        <v>377</v>
+        <v>351</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>378</v>
+        <v>352</v>
       </c>
       <c r="C50" s="20"/>
       <c r="D50" s="20" t="s">
-        <v>379</v>
+        <v>353</v>
       </c>
       <c r="E50" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>133</v>
+        <v>354</v>
       </c>
       <c r="G50" s="22" t="s">
-        <v>134</v>
+        <v>355</v>
       </c>
       <c r="H50" s="20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I50" s="20">
-        <v>4</v>
-      </c>
-      <c r="J50" s="20">
-        <v>43</v>
-      </c>
-      <c r="K50" s="20">
-        <v>2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="J50" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="K50" s="20"/>
       <c r="L50" s="20" t="s">
-        <v>380</v>
+        <v>208</v>
       </c>
       <c r="M50" s="20" t="s">
-        <v>381</v>
+        <v>357</v>
       </c>
       <c r="N50" s="12"/>
       <c r="O50" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P50" s="20" t="s">
-        <v>382</v>
+        <v>358</v>
       </c>
       <c r="Q50" s="20"/>
       <c r="R50" s="20"/>
@@ -4636,50 +4612,46 @@
     </row>
     <row r="51" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>384</v>
-      </c>
-      <c r="C51" s="27" t="s">
-        <v>385</v>
-      </c>
+        <v>360</v>
+      </c>
+      <c r="C51" s="20"/>
       <c r="D51" s="20" t="s">
-        <v>386</v>
+        <v>361</v>
       </c>
       <c r="E51" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F51" s="21" t="s">
-        <v>69</v>
+        <v>362</v>
       </c>
       <c r="G51" s="22" t="s">
-        <v>70</v>
+        <v>363</v>
       </c>
       <c r="H51" s="20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I51" s="20">
-        <v>5</v>
-      </c>
-      <c r="J51" s="20">
-        <v>53</v>
-      </c>
-      <c r="K51" s="23">
-        <v>44198</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="J51" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="K51" s="20"/>
       <c r="L51" s="20" t="s">
-        <v>104</v>
+        <v>208</v>
       </c>
       <c r="M51" s="20" t="s">
-        <v>387</v>
+        <v>364</v>
       </c>
       <c r="N51" s="12"/>
       <c r="O51" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P51" s="20" t="s">
-        <v>388</v>
+        <v>365</v>
       </c>
       <c r="Q51" s="20"/>
       <c r="R51" s="20"/>
@@ -4694,48 +4666,46 @@
     </row>
     <row r="52" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
-        <v>389</v>
+        <v>366</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>390</v>
+        <v>367</v>
       </c>
       <c r="C52" s="20"/>
       <c r="D52" s="20" t="s">
-        <v>391</v>
+        <v>368</v>
       </c>
       <c r="E52" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>392</v>
+        <v>131</v>
       </c>
       <c r="G52" s="22" t="s">
-        <v>393</v>
+        <v>132</v>
       </c>
       <c r="H52" s="20">
         <v>1</v>
       </c>
       <c r="I52" s="20">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J52" s="20">
-        <v>77</v>
-      </c>
-      <c r="K52" s="23">
-        <v>44198</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="K52" s="20"/>
       <c r="L52" s="20" t="s">
-        <v>208</v>
+        <v>45</v>
       </c>
       <c r="M52" s="20" t="s">
-        <v>394</v>
+        <v>369</v>
       </c>
       <c r="N52" s="12"/>
       <c r="O52" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P52" s="20" t="s">
-        <v>395</v>
+        <v>370</v>
       </c>
       <c r="Q52" s="20"/>
       <c r="R52" s="20"/>
@@ -4750,48 +4720,50 @@
     </row>
     <row r="53" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="19" t="s">
-        <v>396</v>
+        <v>371</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>397</v>
-      </c>
-      <c r="C53" s="20"/>
+        <v>372</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>373</v>
+      </c>
       <c r="D53" s="20" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
       <c r="E53" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F53" s="21" t="s">
-        <v>399</v>
+        <v>133</v>
       </c>
       <c r="G53" s="22" t="s">
-        <v>400</v>
+        <v>134</v>
       </c>
       <c r="H53" s="20">
         <v>1</v>
       </c>
       <c r="I53" s="20">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J53" s="20">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="K53" s="20">
         <v>2</v>
       </c>
       <c r="L53" s="20" t="s">
-        <v>188</v>
+        <v>65</v>
       </c>
       <c r="M53" s="20" t="s">
-        <v>401</v>
+        <v>375</v>
       </c>
       <c r="N53" s="12"/>
       <c r="O53" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P53" s="20" t="s">
-        <v>402</v>
+        <v>376</v>
       </c>
       <c r="Q53" s="20"/>
       <c r="R53" s="20"/>
@@ -4806,48 +4778,48 @@
     </row>
     <row r="54" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
-        <v>403</v>
+        <v>377</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>404</v>
+        <v>378</v>
       </c>
       <c r="C54" s="20"/>
       <c r="D54" s="20" t="s">
-        <v>405</v>
+        <v>379</v>
       </c>
       <c r="E54" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>406</v>
+        <v>133</v>
       </c>
       <c r="G54" s="22" t="s">
-        <v>407</v>
+        <v>134</v>
       </c>
       <c r="H54" s="20">
         <v>1</v>
       </c>
       <c r="I54" s="20">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J54" s="20">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="K54" s="20">
         <v>2</v>
       </c>
       <c r="L54" s="20" t="s">
-        <v>408</v>
+        <v>380</v>
       </c>
       <c r="M54" s="20" t="s">
-        <v>409</v>
+        <v>381</v>
       </c>
       <c r="N54" s="12"/>
       <c r="O54" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P54" s="20" t="s">
-        <v>410</v>
+        <v>382</v>
       </c>
       <c r="Q54" s="20"/>
       <c r="R54" s="20"/>
@@ -4862,48 +4834,50 @@
     </row>
     <row r="55" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="s">
-        <v>411</v>
+        <v>383</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>412</v>
-      </c>
-      <c r="C55" s="20"/>
+        <v>384</v>
+      </c>
+      <c r="C55" s="27" t="s">
+        <v>385</v>
+      </c>
       <c r="D55" s="20" t="s">
-        <v>413</v>
+        <v>386</v>
       </c>
       <c r="E55" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F55" s="21" t="s">
-        <v>135</v>
+        <v>69</v>
       </c>
       <c r="G55" s="22" t="s">
-        <v>136</v>
+        <v>70</v>
       </c>
       <c r="H55" s="20">
         <v>1</v>
       </c>
       <c r="I55" s="20">
-        <v>9</v>
-      </c>
-      <c r="J55" s="20" t="s">
-        <v>414</v>
-      </c>
-      <c r="K55" s="20" t="s">
-        <v>140</v>
+        <v>5</v>
+      </c>
+      <c r="J55" s="20">
+        <v>53</v>
+      </c>
+      <c r="K55" s="23">
+        <v>44198</v>
       </c>
       <c r="L55" s="20" t="s">
-        <v>415</v>
+        <v>104</v>
       </c>
       <c r="M55" s="20" t="s">
-        <v>416</v>
+        <v>387</v>
       </c>
       <c r="N55" s="12"/>
       <c r="O55" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P55" s="20" t="s">
-        <v>417</v>
+        <v>388</v>
       </c>
       <c r="Q55" s="20"/>
       <c r="R55" s="20"/>
@@ -4918,32 +4892,32 @@
     </row>
     <row r="56" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
-        <v>418</v>
+        <v>389</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>419</v>
+        <v>390</v>
       </c>
       <c r="C56" s="20"/>
       <c r="D56" s="20" t="s">
-        <v>420</v>
+        <v>391</v>
       </c>
       <c r="E56" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F56" s="21" t="s">
-        <v>66</v>
+        <v>392</v>
       </c>
       <c r="G56" s="22" t="s">
-        <v>67</v>
+        <v>393</v>
       </c>
       <c r="H56" s="20">
         <v>1</v>
       </c>
       <c r="I56" s="20">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="J56" s="20">
-        <v>124</v>
+        <v>77</v>
       </c>
       <c r="K56" s="23">
         <v>44198</v>
@@ -4952,14 +4926,14 @@
         <v>208</v>
       </c>
       <c r="M56" s="20" t="s">
-        <v>421</v>
+        <v>394</v>
       </c>
       <c r="N56" s="12"/>
       <c r="O56" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P56" s="20" t="s">
-        <v>422</v>
+        <v>395</v>
       </c>
       <c r="Q56" s="20"/>
       <c r="R56" s="20"/>
@@ -4974,48 +4948,48 @@
     </row>
     <row r="57" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
-        <v>423</v>
+        <v>396</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>378</v>
+        <v>397</v>
       </c>
       <c r="C57" s="20"/>
       <c r="D57" s="20" t="s">
-        <v>379</v>
+        <v>398</v>
       </c>
       <c r="E57" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F57" s="21" t="s">
-        <v>66</v>
+        <v>399</v>
       </c>
       <c r="G57" s="22" t="s">
-        <v>67</v>
+        <v>400</v>
       </c>
       <c r="H57" s="20">
         <v>1</v>
       </c>
       <c r="I57" s="20">
-        <v>11</v>
-      </c>
-      <c r="J57" s="20" t="s">
-        <v>347</v>
+        <v>8</v>
+      </c>
+      <c r="J57" s="20">
+        <v>88</v>
       </c>
       <c r="K57" s="20">
         <v>2</v>
       </c>
       <c r="L57" s="20" t="s">
-        <v>380</v>
+        <v>188</v>
       </c>
       <c r="M57" s="20" t="s">
-        <v>424</v>
+        <v>401</v>
       </c>
       <c r="N57" s="12"/>
       <c r="O57" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P57" s="20" t="s">
-        <v>425</v>
+        <v>402</v>
       </c>
       <c r="Q57" s="20"/>
       <c r="R57" s="20"/>
@@ -5030,48 +5004,48 @@
     </row>
     <row r="58" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
-        <v>426</v>
+        <v>403</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>42</v>
+        <v>404</v>
       </c>
       <c r="C58" s="20"/>
       <c r="D58" s="20" t="s">
-        <v>427</v>
+        <v>405</v>
       </c>
       <c r="E58" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F58" s="21" t="s">
-        <v>66</v>
+        <v>406</v>
       </c>
       <c r="G58" s="22" t="s">
-        <v>67</v>
+        <v>407</v>
       </c>
       <c r="H58" s="20">
         <v>1</v>
       </c>
       <c r="I58" s="20">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="J58" s="20">
-        <v>131</v>
+        <v>65</v>
       </c>
       <c r="K58" s="20">
         <v>2</v>
       </c>
       <c r="L58" s="20" t="s">
-        <v>208</v>
+        <v>408</v>
       </c>
       <c r="M58" s="20" t="s">
-        <v>428</v>
+        <v>409</v>
       </c>
       <c r="N58" s="12"/>
       <c r="O58" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P58" s="20" t="s">
-        <v>429</v>
+        <v>410</v>
       </c>
       <c r="Q58" s="20"/>
       <c r="R58" s="20"/>
@@ -5086,48 +5060,48 @@
     </row>
     <row r="59" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="s">
-        <v>430</v>
+        <v>411</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>431</v>
+        <v>412</v>
       </c>
       <c r="C59" s="20"/>
       <c r="D59" s="20" t="s">
-        <v>432</v>
+        <v>413</v>
       </c>
       <c r="E59" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F59" s="21" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="G59" s="22" t="s">
-        <v>74</v>
+        <v>136</v>
       </c>
       <c r="H59" s="20">
         <v>1</v>
       </c>
       <c r="I59" s="20">
-        <v>12</v>
-      </c>
-      <c r="J59" s="20">
-        <v>136</v>
-      </c>
-      <c r="K59" s="20">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="J59" s="20" t="s">
+        <v>414</v>
+      </c>
+      <c r="K59" s="20" t="s">
+        <v>140</v>
       </c>
       <c r="L59" s="20" t="s">
-        <v>208</v>
+        <v>415</v>
       </c>
       <c r="M59" s="20" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="N59" s="12"/>
       <c r="O59" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P59" s="20" t="s">
-        <v>434</v>
+        <v>417</v>
       </c>
       <c r="Q59" s="20"/>
       <c r="R59" s="20"/>
@@ -5142,48 +5116,48 @@
     </row>
     <row r="60" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="s">
-        <v>435</v>
+        <v>418</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>436</v>
+        <v>419</v>
       </c>
       <c r="C60" s="20"/>
       <c r="D60" s="20" t="s">
-        <v>437</v>
+        <v>420</v>
       </c>
       <c r="E60" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F60" s="21" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G60" s="22" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="H60" s="20">
         <v>1</v>
       </c>
       <c r="I60" s="20">
-        <v>12</v>
-      </c>
-      <c r="J60" s="20" t="s">
-        <v>438</v>
-      </c>
-      <c r="K60" s="20" t="s">
-        <v>439</v>
+        <v>11</v>
+      </c>
+      <c r="J60" s="20">
+        <v>124</v>
+      </c>
+      <c r="K60" s="23">
+        <v>44198</v>
       </c>
       <c r="L60" s="20" t="s">
         <v>208</v>
       </c>
       <c r="M60" s="20" t="s">
-        <v>440</v>
+        <v>421</v>
       </c>
       <c r="N60" s="12"/>
       <c r="O60" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P60" s="20" t="s">
-        <v>441</v>
+        <v>422</v>
       </c>
       <c r="Q60" s="20"/>
       <c r="R60" s="20"/>
@@ -5198,48 +5172,48 @@
     </row>
     <row r="61" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A61" s="19" t="s">
-        <v>442</v>
+        <v>423</v>
       </c>
       <c r="B61" s="20" t="s">
-        <v>443</v>
+        <v>378</v>
       </c>
       <c r="C61" s="20"/>
       <c r="D61" s="20" t="s">
-        <v>444</v>
+        <v>379</v>
       </c>
       <c r="E61" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F61" s="21" t="s">
-        <v>138</v>
+        <v>66</v>
       </c>
       <c r="G61" s="22" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="H61" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I61" s="20">
-        <v>13</v>
-      </c>
-      <c r="J61" s="20">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="J61" s="20" t="s">
+        <v>347</v>
       </c>
       <c r="K61" s="20">
         <v>2</v>
       </c>
       <c r="L61" s="20" t="s">
-        <v>208</v>
+        <v>380</v>
       </c>
       <c r="M61" s="20" t="s">
-        <v>445</v>
+        <v>424</v>
       </c>
       <c r="N61" s="12"/>
       <c r="O61" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P61" s="20" t="s">
-        <v>446</v>
+        <v>425</v>
       </c>
       <c r="Q61" s="20"/>
       <c r="R61" s="20"/>
@@ -5254,48 +5228,48 @@
     </row>
     <row r="62" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A62" s="19" t="s">
-        <v>447</v>
+        <v>426</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>448</v>
+        <v>42</v>
       </c>
       <c r="C62" s="20"/>
       <c r="D62" s="20" t="s">
-        <v>449</v>
+        <v>427</v>
       </c>
       <c r="E62" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F62" s="21" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="G62" s="22" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="H62" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I62" s="20">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J62" s="20">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="K62" s="20">
         <v>2</v>
       </c>
       <c r="L62" s="20" t="s">
-        <v>45</v>
+        <v>208</v>
       </c>
       <c r="M62" s="20" t="s">
-        <v>450</v>
+        <v>428</v>
       </c>
       <c r="N62" s="12"/>
       <c r="O62" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P62" s="20" t="s">
-        <v>451</v>
+        <v>429</v>
       </c>
       <c r="Q62" s="20"/>
       <c r="R62" s="20"/>
@@ -5310,48 +5284,48 @@
     </row>
     <row r="63" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" s="19" t="s">
-        <v>452</v>
+        <v>430</v>
       </c>
       <c r="B63" s="20" t="s">
-        <v>453</v>
+        <v>431</v>
       </c>
       <c r="C63" s="20"/>
       <c r="D63" s="20" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="E63" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F63" s="21" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="H63" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I63" s="20">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J63" s="20">
-        <v>13</v>
+        <v>136</v>
       </c>
       <c r="K63" s="20">
         <v>2</v>
       </c>
       <c r="L63" s="20" t="s">
-        <v>45</v>
+        <v>208</v>
       </c>
       <c r="M63" s="20" t="s">
-        <v>455</v>
+        <v>433</v>
       </c>
       <c r="N63" s="12"/>
       <c r="O63" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P63" s="20" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="Q63" s="20"/>
       <c r="R63" s="20"/>
@@ -5366,48 +5340,48 @@
     </row>
     <row r="64" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A64" s="19" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
       <c r="C64" s="20"/>
       <c r="D64" s="20" t="s">
-        <v>459</v>
+        <v>437</v>
       </c>
       <c r="E64" s="20" t="s">
         <v>189</v>
       </c>
       <c r="F64" s="21" t="s">
-        <v>141</v>
+        <v>73</v>
       </c>
       <c r="G64" s="22" t="s">
-        <v>142</v>
+        <v>74</v>
       </c>
       <c r="H64" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I64" s="20">
-        <v>15</v>
-      </c>
-      <c r="J64" s="20">
-        <v>26</v>
-      </c>
-      <c r="K64" s="20">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="J64" s="20" t="s">
+        <v>438</v>
+      </c>
+      <c r="K64" s="20" t="s">
+        <v>439</v>
       </c>
       <c r="L64" s="20" t="s">
-        <v>45</v>
+        <v>208</v>
       </c>
       <c r="M64" s="20" t="s">
-        <v>460</v>
+        <v>440</v>
       </c>
       <c r="N64" s="12"/>
       <c r="O64" s="20" t="s">
         <v>193</v>
       </c>
       <c r="P64" s="20" t="s">
-        <v>461</v>
+        <v>441</v>
       </c>
       <c r="Q64" s="20"/>
       <c r="R64" s="20"/>
@@ -5421,270 +5395,394 @@
       <c r="Z64" s="24"/>
     </row>
     <row r="65" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A65" s="28" t="s">
+      <c r="A65" s="19" t="s">
+        <v>442</v>
+      </c>
+      <c r="B65" s="20" t="s">
+        <v>443</v>
+      </c>
+      <c r="C65" s="20"/>
+      <c r="D65" s="20" t="s">
+        <v>444</v>
+      </c>
+      <c r="E65" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="F65" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="G65" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="H65" s="20">
+        <v>2</v>
+      </c>
+      <c r="I65" s="20">
+        <v>13</v>
+      </c>
+      <c r="J65" s="20">
+        <v>9</v>
+      </c>
+      <c r="K65" s="20">
+        <v>2</v>
+      </c>
+      <c r="L65" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="M65" s="20" t="s">
+        <v>445</v>
+      </c>
+      <c r="N65" s="12"/>
+      <c r="O65" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="P65" s="20" t="s">
+        <v>446</v>
+      </c>
+      <c r="Q65" s="20"/>
+      <c r="R65" s="20"/>
+      <c r="S65" s="20"/>
+      <c r="T65" s="20"/>
+      <c r="U65" s="20"/>
+      <c r="V65" s="20"/>
+      <c r="W65" s="24"/>
+      <c r="X65" s="24"/>
+      <c r="Y65" s="24"/>
+      <c r="Z65" s="24"/>
+    </row>
+    <row r="66" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A66" s="19" t="s">
+        <v>447</v>
+      </c>
+      <c r="B66" s="20" t="s">
+        <v>448</v>
+      </c>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20" t="s">
+        <v>449</v>
+      </c>
+      <c r="E66" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="F66" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="G66" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="H66" s="20">
+        <v>2</v>
+      </c>
+      <c r="I66" s="20">
+        <v>14</v>
+      </c>
+      <c r="J66" s="20">
+        <v>20</v>
+      </c>
+      <c r="K66" s="20">
+        <v>2</v>
+      </c>
+      <c r="L66" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="M66" s="20" t="s">
+        <v>450</v>
+      </c>
+      <c r="N66" s="12"/>
+      <c r="O66" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="P66" s="20" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q66" s="20"/>
+      <c r="R66" s="20"/>
+      <c r="S66" s="20"/>
+      <c r="T66" s="20"/>
+      <c r="U66" s="20"/>
+      <c r="V66" s="20"/>
+      <c r="W66" s="24"/>
+      <c r="X66" s="24"/>
+      <c r="Y66" s="24"/>
+      <c r="Z66" s="24"/>
+    </row>
+    <row r="67" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A67" s="19" t="s">
+        <v>452</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>453</v>
+      </c>
+      <c r="C67" s="20"/>
+      <c r="D67" s="20" t="s">
+        <v>454</v>
+      </c>
+      <c r="E67" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="F67" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="G67" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="H67" s="20">
+        <v>2</v>
+      </c>
+      <c r="I67" s="20">
+        <v>14</v>
+      </c>
+      <c r="J67" s="20">
+        <v>13</v>
+      </c>
+      <c r="K67" s="20">
+        <v>2</v>
+      </c>
+      <c r="L67" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="M67" s="20" t="s">
+        <v>455</v>
+      </c>
+      <c r="N67" s="12"/>
+      <c r="O67" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="P67" s="20" t="s">
+        <v>456</v>
+      </c>
+      <c r="Q67" s="20"/>
+      <c r="R67" s="20"/>
+      <c r="S67" s="20"/>
+      <c r="T67" s="20"/>
+      <c r="U67" s="20"/>
+      <c r="V67" s="20"/>
+      <c r="W67" s="24"/>
+      <c r="X67" s="24"/>
+      <c r="Y67" s="24"/>
+      <c r="Z67" s="24"/>
+    </row>
+    <row r="68" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A68" s="19" t="s">
+        <v>457</v>
+      </c>
+      <c r="B68" s="20" t="s">
+        <v>458</v>
+      </c>
+      <c r="C68" s="20"/>
+      <c r="D68" s="20" t="s">
+        <v>459</v>
+      </c>
+      <c r="E68" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="F68" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="G68" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="H68" s="20">
+        <v>2</v>
+      </c>
+      <c r="I68" s="20">
+        <v>15</v>
+      </c>
+      <c r="J68" s="20">
+        <v>26</v>
+      </c>
+      <c r="K68" s="20">
+        <v>2</v>
+      </c>
+      <c r="L68" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="M68" s="20" t="s">
+        <v>460</v>
+      </c>
+      <c r="N68" s="12"/>
+      <c r="O68" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="P68" s="20" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q68" s="20"/>
+      <c r="R68" s="20"/>
+      <c r="S68" s="20"/>
+      <c r="T68" s="20"/>
+      <c r="U68" s="20"/>
+      <c r="V68" s="20"/>
+      <c r="W68" s="24"/>
+      <c r="X68" s="24"/>
+      <c r="Y68" s="24"/>
+      <c r="Z68" s="24"/>
+    </row>
+    <row r="69" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A69" s="28" t="s">
         <v>462</v>
       </c>
-      <c r="B65" s="29" t="s">
+      <c r="B69" s="29" t="s">
         <v>390</v>
       </c>
-      <c r="C65" s="29"/>
-      <c r="D65" s="29" t="s">
+      <c r="C69" s="29"/>
+      <c r="D69" s="29" t="s">
         <v>463</v>
       </c>
-      <c r="E65" s="29" t="s">
+      <c r="E69" s="29" t="s">
         <v>189</v>
       </c>
-      <c r="F65" s="30" t="s">
+      <c r="F69" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="G65" s="31" t="s">
+      <c r="G69" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="H65" s="29">
+      <c r="H69" s="29">
         <v>2</v>
       </c>
-      <c r="I65" s="29">
+      <c r="I69" s="29">
         <v>15</v>
       </c>
-      <c r="J65" s="29" t="s">
+      <c r="J69" s="29" t="s">
         <v>464</v>
       </c>
-      <c r="K65" s="29" t="s">
+      <c r="K69" s="29" t="s">
         <v>439</v>
       </c>
-      <c r="L65" s="29" t="s">
+      <c r="L69" s="29" t="s">
         <v>208</v>
       </c>
-      <c r="M65" s="29" t="s">
+      <c r="M69" s="29" t="s">
         <v>465</v>
       </c>
-      <c r="N65" s="12"/>
-      <c r="O65" s="29" t="s">
+      <c r="N69" s="12"/>
+      <c r="O69" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="P65" s="29" t="s">
+      <c r="P69" s="29" t="s">
         <v>466</v>
       </c>
-      <c r="Q65" s="29"/>
-      <c r="R65" s="29"/>
-      <c r="S65" s="29"/>
-      <c r="T65" s="29"/>
-      <c r="U65" s="29"/>
-      <c r="V65" s="29"/>
-      <c r="W65" s="32"/>
-      <c r="X65" s="32"/>
-      <c r="Y65" s="32"/>
-      <c r="Z65" s="32"/>
-    </row>
-    <row r="66" spans="1:26" s="36" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A66" s="33" t="s">
+      <c r="Q69" s="29"/>
+      <c r="R69" s="29"/>
+      <c r="S69" s="29"/>
+      <c r="T69" s="29"/>
+      <c r="U69" s="29"/>
+      <c r="V69" s="29"/>
+      <c r="W69" s="32"/>
+      <c r="X69" s="32"/>
+      <c r="Y69" s="32"/>
+      <c r="Z69" s="32"/>
+    </row>
+    <row r="70" spans="1:26" s="36" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A70" s="33" t="s">
         <v>467</v>
       </c>
-      <c r="B66" s="34" t="s">
+      <c r="B70" s="34" t="s">
         <v>468</v>
       </c>
-      <c r="C66" s="34"/>
-      <c r="D66" s="34" t="s">
+      <c r="C70" s="34"/>
+      <c r="D70" s="34" t="s">
         <v>469</v>
       </c>
-      <c r="E66" s="34" t="s">
+      <c r="E70" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="F66" s="34" t="s">
+      <c r="F70" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="G66" s="34" t="s">
+      <c r="G70" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="H66" s="34">
+      <c r="H70" s="34">
         <v>2</v>
       </c>
-      <c r="I66" s="34">
+      <c r="I70" s="34">
         <v>16</v>
       </c>
-      <c r="J66" s="34" t="s">
+      <c r="J70" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="K66" s="35"/>
-      <c r="L66" s="34" t="s">
+      <c r="K70" s="35"/>
+      <c r="L70" s="34" t="s">
         <v>208</v>
       </c>
-      <c r="M66" s="34" t="s">
+      <c r="M70" s="34" t="s">
         <v>470</v>
       </c>
-      <c r="N66" s="12"/>
-      <c r="O66" s="34" t="s">
+      <c r="N70" s="12"/>
+      <c r="O70" s="34" t="s">
         <v>193</v>
       </c>
-      <c r="P66" s="34" t="s">
+      <c r="P70" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="Q66" s="35"/>
-      <c r="R66" s="35"/>
-      <c r="S66" s="35"/>
-      <c r="T66" s="35"/>
-      <c r="U66" s="35"/>
-      <c r="V66" s="35"/>
-      <c r="W66" s="35"/>
-      <c r="X66" s="35"/>
-      <c r="Y66" s="35"/>
-      <c r="Z66" s="35"/>
-    </row>
-    <row r="67" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A67" s="37" t="s">
+      <c r="Q70" s="35"/>
+      <c r="R70" s="35"/>
+      <c r="S70" s="35"/>
+      <c r="T70" s="35"/>
+      <c r="U70" s="35"/>
+      <c r="V70" s="35"/>
+      <c r="W70" s="35"/>
+      <c r="X70" s="35"/>
+      <c r="Y70" s="35"/>
+      <c r="Z70" s="35"/>
+    </row>
+    <row r="71" spans="1:26" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A71" s="37" t="s">
         <v>472</v>
       </c>
-      <c r="B67" s="38" t="s">
+      <c r="B71" s="38" t="s">
         <v>473</v>
       </c>
-      <c r="C67" s="38"/>
-      <c r="D67" s="39" t="s">
+      <c r="C71" s="38"/>
+      <c r="D71" s="39" t="s">
         <v>474</v>
       </c>
-      <c r="E67" s="38" t="s">
+      <c r="E71" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="F67" s="40" t="s">
+      <c r="F71" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="G67" s="41" t="s">
+      <c r="G71" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="H67" s="38">
+      <c r="H71" s="38">
         <v>2</v>
       </c>
-      <c r="I67" s="38">
+      <c r="I71" s="38">
         <v>16</v>
       </c>
-      <c r="J67" s="38">
+      <c r="J71" s="38">
         <v>41</v>
       </c>
-      <c r="K67" s="38">
+      <c r="K71" s="38">
         <v>2</v>
       </c>
-      <c r="L67" s="38" t="s">
+      <c r="L71" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="M67" s="38" t="s">
+      <c r="M71" s="38" t="s">
         <v>475</v>
       </c>
-      <c r="N67" s="12"/>
-      <c r="O67" s="38" t="s">
+      <c r="N71" s="12"/>
+      <c r="O71" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="P67" s="38" t="s">
+      <c r="P71" s="38" t="s">
         <v>476</v>
       </c>
-      <c r="Q67" s="38"/>
-      <c r="R67" s="38"/>
-      <c r="S67" s="38"/>
-      <c r="T67" s="38"/>
-      <c r="U67" s="38"/>
-      <c r="V67" s="38"/>
-      <c r="W67" s="42"/>
-      <c r="X67" s="42"/>
-      <c r="Y67" s="42"/>
-      <c r="Z67" s="42"/>
-    </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A68" s="7"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
-      <c r="E68" s="7"/>
-      <c r="F68" s="8"/>
-      <c r="G68" s="7"/>
-      <c r="H68" s="7"/>
-      <c r="I68" s="7"/>
-      <c r="J68" s="7"/>
-      <c r="K68" s="7"/>
-      <c r="L68" s="7"/>
-      <c r="M68" s="7"/>
-      <c r="N68" s="12"/>
-      <c r="O68" s="5"/>
-      <c r="P68" s="5"/>
-      <c r="Q68" s="5"/>
-      <c r="R68" s="5"/>
-      <c r="S68" s="5"/>
-      <c r="T68" s="5"/>
-      <c r="U68" s="5"/>
-      <c r="V68" s="5"/>
-      <c r="W68" s="5"/>
-    </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A69" s="7"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="7"/>
-      <c r="D69" s="7"/>
-      <c r="E69" s="7"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="7"/>
-      <c r="H69" s="7"/>
-      <c r="I69" s="7"/>
-      <c r="J69" s="7"/>
-      <c r="K69" s="7"/>
-      <c r="L69" s="7"/>
-      <c r="M69" s="7"/>
-      <c r="N69" s="12"/>
-      <c r="O69" s="5"/>
-      <c r="P69" s="5"/>
-      <c r="Q69" s="5"/>
-      <c r="R69" s="5"/>
-      <c r="S69" s="5"/>
-      <c r="T69" s="5"/>
-      <c r="U69" s="5"/>
-      <c r="V69" s="5"/>
-      <c r="W69" s="5"/>
-    </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A70" s="7"/>
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="8"/>
-      <c r="G70" s="7"/>
-      <c r="H70" s="7"/>
-      <c r="I70" s="7"/>
-      <c r="J70" s="7"/>
-      <c r="K70" s="7"/>
-      <c r="L70" s="7"/>
-      <c r="M70" s="7"/>
-      <c r="N70" s="12"/>
-      <c r="O70" s="5"/>
-      <c r="P70" s="5"/>
-      <c r="Q70" s="5"/>
-      <c r="R70" s="5"/>
-      <c r="S70" s="5"/>
-      <c r="T70" s="5"/>
-      <c r="U70" s="5"/>
-      <c r="V70" s="5"/>
-      <c r="W70" s="5"/>
-    </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A71" s="7"/>
-      <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="8"/>
-      <c r="G71" s="7"/>
-      <c r="H71" s="7"/>
-      <c r="I71" s="7"/>
-      <c r="J71" s="7"/>
-      <c r="K71" s="7"/>
-      <c r="L71" s="7"/>
-      <c r="M71" s="7"/>
-      <c r="N71" s="12"/>
-      <c r="O71" s="5"/>
-      <c r="P71" s="5"/>
-      <c r="Q71" s="5"/>
-      <c r="R71" s="5"/>
-      <c r="S71" s="5"/>
-      <c r="T71" s="5"/>
-      <c r="U71" s="5"/>
-      <c r="V71" s="5"/>
-      <c r="W71" s="5"/>
+      <c r="Q71" s="38"/>
+      <c r="R71" s="38"/>
+      <c r="S71" s="38"/>
+      <c r="T71" s="38"/>
+      <c r="U71" s="38"/>
+      <c r="V71" s="38"/>
+      <c r="W71" s="42"/>
+      <c r="X71" s="42"/>
+      <c r="Y71" s="42"/>
+      <c r="Z71" s="42"/>
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A72" s="7"/>
@@ -5750,7 +5848,7 @@
       <c r="K74" s="7"/>
       <c r="L74" s="7"/>
       <c r="M74" s="7"/>
-      <c r="N74" s="7"/>
+      <c r="N74" s="12"/>
       <c r="O74" s="5"/>
       <c r="P74" s="5"/>
       <c r="Q74" s="5"/>
@@ -5775,7 +5873,7 @@
       <c r="K75" s="7"/>
       <c r="L75" s="7"/>
       <c r="M75" s="7"/>
-      <c r="N75" s="7"/>
+      <c r="N75" s="12"/>
       <c r="O75" s="5"/>
       <c r="P75" s="5"/>
       <c r="Q75" s="5"/>
@@ -5800,7 +5898,7 @@
       <c r="K76" s="7"/>
       <c r="L76" s="7"/>
       <c r="M76" s="7"/>
-      <c r="N76" s="7"/>
+      <c r="N76" s="12"/>
       <c r="O76" s="5"/>
       <c r="P76" s="5"/>
       <c r="Q76" s="5"/>
@@ -5825,7 +5923,7 @@
       <c r="K77" s="7"/>
       <c r="L77" s="7"/>
       <c r="M77" s="7"/>
-      <c r="N77" s="7"/>
+      <c r="N77" s="12"/>
       <c r="O77" s="5"/>
       <c r="P77" s="5"/>
       <c r="Q77" s="5"/>
@@ -21887,104 +21985,104 @@
       <c r="W719" s="5"/>
     </row>
     <row r="720" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A720" s="1"/>
-      <c r="B720" s="1"/>
-      <c r="C720" s="1"/>
-      <c r="D720" s="1"/>
-      <c r="E720" s="1"/>
-      <c r="F720" s="1"/>
-      <c r="G720" s="1"/>
-      <c r="H720" s="1"/>
-      <c r="I720" s="1"/>
-      <c r="J720" s="1"/>
-      <c r="K720" s="1"/>
-      <c r="L720" s="1"/>
-      <c r="M720" s="10"/>
-      <c r="N720" s="1"/>
-      <c r="O720" s="1"/>
-      <c r="P720" s="1"/>
-      <c r="Q720" s="1"/>
-      <c r="R720" s="1"/>
-      <c r="S720" s="1"/>
-      <c r="T720" s="1"/>
-      <c r="U720" s="1"/>
-      <c r="V720" s="1"/>
-      <c r="W720" s="1"/>
+      <c r="A720" s="7"/>
+      <c r="B720" s="7"/>
+      <c r="C720" s="7"/>
+      <c r="D720" s="7"/>
+      <c r="E720" s="7"/>
+      <c r="F720" s="8"/>
+      <c r="G720" s="7"/>
+      <c r="H720" s="7"/>
+      <c r="I720" s="7"/>
+      <c r="J720" s="7"/>
+      <c r="K720" s="7"/>
+      <c r="L720" s="7"/>
+      <c r="M720" s="7"/>
+      <c r="N720" s="7"/>
+      <c r="O720" s="5"/>
+      <c r="P720" s="5"/>
+      <c r="Q720" s="5"/>
+      <c r="R720" s="5"/>
+      <c r="S720" s="5"/>
+      <c r="T720" s="5"/>
+      <c r="U720" s="5"/>
+      <c r="V720" s="5"/>
+      <c r="W720" s="5"/>
     </row>
     <row r="721" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A721" s="1"/>
-      <c r="B721" s="1"/>
-      <c r="C721" s="1"/>
-      <c r="D721" s="1"/>
-      <c r="E721" s="1"/>
-      <c r="F721" s="1"/>
-      <c r="G721" s="1"/>
-      <c r="H721" s="1"/>
-      <c r="I721" s="1"/>
-      <c r="J721" s="1"/>
-      <c r="K721" s="1"/>
-      <c r="L721" s="1"/>
-      <c r="M721" s="10"/>
-      <c r="N721" s="1"/>
-      <c r="O721" s="1"/>
-      <c r="P721" s="1"/>
-      <c r="Q721" s="1"/>
-      <c r="R721" s="1"/>
-      <c r="S721" s="1"/>
-      <c r="T721" s="1"/>
-      <c r="U721" s="1"/>
-      <c r="V721" s="1"/>
-      <c r="W721" s="1"/>
+      <c r="A721" s="7"/>
+      <c r="B721" s="7"/>
+      <c r="C721" s="7"/>
+      <c r="D721" s="7"/>
+      <c r="E721" s="7"/>
+      <c r="F721" s="8"/>
+      <c r="G721" s="7"/>
+      <c r="H721" s="7"/>
+      <c r="I721" s="7"/>
+      <c r="J721" s="7"/>
+      <c r="K721" s="7"/>
+      <c r="L721" s="7"/>
+      <c r="M721" s="7"/>
+      <c r="N721" s="7"/>
+      <c r="O721" s="5"/>
+      <c r="P721" s="5"/>
+      <c r="Q721" s="5"/>
+      <c r="R721" s="5"/>
+      <c r="S721" s="5"/>
+      <c r="T721" s="5"/>
+      <c r="U721" s="5"/>
+      <c r="V721" s="5"/>
+      <c r="W721" s="5"/>
     </row>
     <row r="722" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A722" s="1"/>
-      <c r="B722" s="1"/>
-      <c r="C722" s="1"/>
-      <c r="D722" s="1"/>
-      <c r="E722" s="1"/>
-      <c r="F722" s="1"/>
-      <c r="G722" s="1"/>
-      <c r="H722" s="1"/>
-      <c r="I722" s="1"/>
-      <c r="J722" s="1"/>
-      <c r="K722" s="1"/>
-      <c r="L722" s="1"/>
-      <c r="M722" s="10"/>
-      <c r="N722" s="1"/>
-      <c r="O722" s="1"/>
-      <c r="P722" s="1"/>
-      <c r="Q722" s="1"/>
-      <c r="R722" s="1"/>
-      <c r="S722" s="1"/>
-      <c r="T722" s="1"/>
-      <c r="U722" s="1"/>
-      <c r="V722" s="1"/>
-      <c r="W722" s="1"/>
+      <c r="A722" s="7"/>
+      <c r="B722" s="7"/>
+      <c r="C722" s="7"/>
+      <c r="D722" s="7"/>
+      <c r="E722" s="7"/>
+      <c r="F722" s="8"/>
+      <c r="G722" s="7"/>
+      <c r="H722" s="7"/>
+      <c r="I722" s="7"/>
+      <c r="J722" s="7"/>
+      <c r="K722" s="7"/>
+      <c r="L722" s="7"/>
+      <c r="M722" s="7"/>
+      <c r="N722" s="7"/>
+      <c r="O722" s="5"/>
+      <c r="P722" s="5"/>
+      <c r="Q722" s="5"/>
+      <c r="R722" s="5"/>
+      <c r="S722" s="5"/>
+      <c r="T722" s="5"/>
+      <c r="U722" s="5"/>
+      <c r="V722" s="5"/>
+      <c r="W722" s="5"/>
     </row>
     <row r="723" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A723" s="1"/>
-      <c r="B723" s="1"/>
-      <c r="C723" s="1"/>
-      <c r="D723" s="1"/>
-      <c r="E723" s="1"/>
-      <c r="F723" s="1"/>
-      <c r="G723" s="1"/>
-      <c r="H723" s="1"/>
-      <c r="I723" s="1"/>
-      <c r="J723" s="1"/>
-      <c r="K723" s="1"/>
-      <c r="L723" s="1"/>
-      <c r="M723" s="10"/>
-      <c r="N723" s="1"/>
-      <c r="O723" s="1"/>
-      <c r="P723" s="1"/>
-      <c r="Q723" s="1"/>
-      <c r="R723" s="1"/>
-      <c r="S723" s="1"/>
-      <c r="T723" s="1"/>
-      <c r="U723" s="1"/>
-      <c r="V723" s="1"/>
-      <c r="W723" s="1"/>
+      <c r="A723" s="7"/>
+      <c r="B723" s="7"/>
+      <c r="C723" s="7"/>
+      <c r="D723" s="7"/>
+      <c r="E723" s="7"/>
+      <c r="F723" s="8"/>
+      <c r="G723" s="7"/>
+      <c r="H723" s="7"/>
+      <c r="I723" s="7"/>
+      <c r="J723" s="7"/>
+      <c r="K723" s="7"/>
+      <c r="L723" s="7"/>
+      <c r="M723" s="7"/>
+      <c r="N723" s="7"/>
+      <c r="O723" s="5"/>
+      <c r="P723" s="5"/>
+      <c r="Q723" s="5"/>
+      <c r="R723" s="5"/>
+      <c r="S723" s="5"/>
+      <c r="T723" s="5"/>
+      <c r="U723" s="5"/>
+      <c r="V723" s="5"/>
+      <c r="W723" s="5"/>
     </row>
     <row r="724" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A724" s="1"/>
@@ -22186,6 +22284,106 @@
       <c r="V731" s="1"/>
       <c r="W731" s="1"/>
     </row>
+    <row r="732" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A732" s="1"/>
+      <c r="B732" s="1"/>
+      <c r="C732" s="1"/>
+      <c r="D732" s="1"/>
+      <c r="E732" s="1"/>
+      <c r="F732" s="1"/>
+      <c r="G732" s="1"/>
+      <c r="H732" s="1"/>
+      <c r="I732" s="1"/>
+      <c r="J732" s="1"/>
+      <c r="K732" s="1"/>
+      <c r="L732" s="1"/>
+      <c r="M732" s="10"/>
+      <c r="N732" s="1"/>
+      <c r="O732" s="1"/>
+      <c r="P732" s="1"/>
+      <c r="Q732" s="1"/>
+      <c r="R732" s="1"/>
+      <c r="S732" s="1"/>
+      <c r="T732" s="1"/>
+      <c r="U732" s="1"/>
+      <c r="V732" s="1"/>
+      <c r="W732" s="1"/>
+    </row>
+    <row r="733" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A733" s="1"/>
+      <c r="B733" s="1"/>
+      <c r="C733" s="1"/>
+      <c r="D733" s="1"/>
+      <c r="E733" s="1"/>
+      <c r="F733" s="1"/>
+      <c r="G733" s="1"/>
+      <c r="H733" s="1"/>
+      <c r="I733" s="1"/>
+      <c r="J733" s="1"/>
+      <c r="K733" s="1"/>
+      <c r="L733" s="1"/>
+      <c r="M733" s="10"/>
+      <c r="N733" s="1"/>
+      <c r="O733" s="1"/>
+      <c r="P733" s="1"/>
+      <c r="Q733" s="1"/>
+      <c r="R733" s="1"/>
+      <c r="S733" s="1"/>
+      <c r="T733" s="1"/>
+      <c r="U733" s="1"/>
+      <c r="V733" s="1"/>
+      <c r="W733" s="1"/>
+    </row>
+    <row r="734" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A734" s="1"/>
+      <c r="B734" s="1"/>
+      <c r="C734" s="1"/>
+      <c r="D734" s="1"/>
+      <c r="E734" s="1"/>
+      <c r="F734" s="1"/>
+      <c r="G734" s="1"/>
+      <c r="H734" s="1"/>
+      <c r="I734" s="1"/>
+      <c r="J734" s="1"/>
+      <c r="K734" s="1"/>
+      <c r="L734" s="1"/>
+      <c r="M734" s="10"/>
+      <c r="N734" s="1"/>
+      <c r="O734" s="1"/>
+      <c r="P734" s="1"/>
+      <c r="Q734" s="1"/>
+      <c r="R734" s="1"/>
+      <c r="S734" s="1"/>
+      <c r="T734" s="1"/>
+      <c r="U734" s="1"/>
+      <c r="V734" s="1"/>
+      <c r="W734" s="1"/>
+    </row>
+    <row r="735" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A735" s="1"/>
+      <c r="B735" s="1"/>
+      <c r="C735" s="1"/>
+      <c r="D735" s="1"/>
+      <c r="E735" s="1"/>
+      <c r="F735" s="1"/>
+      <c r="G735" s="1"/>
+      <c r="H735" s="1"/>
+      <c r="I735" s="1"/>
+      <c r="J735" s="1"/>
+      <c r="K735" s="1"/>
+      <c r="L735" s="1"/>
+      <c r="M735" s="10"/>
+      <c r="N735" s="1"/>
+      <c r="O735" s="1"/>
+      <c r="P735" s="1"/>
+      <c r="Q735" s="1"/>
+      <c r="R735" s="1"/>
+      <c r="S735" s="1"/>
+      <c r="T735" s="1"/>
+      <c r="U735" s="1"/>
+      <c r="V735" s="1"/>
+      <c r="W735" s="1"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:W22">
     <sortCondition ref="A4:A22"/>

</xml_diff>